<commit_message>
update model and data
</commit_message>
<xml_diff>
--- a/Code/governance/site-key.xlsx
+++ b/Code/governance/site-key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthipsey/Local/lake-richmond/Code/governance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2DC037-4A28-044B-816F-7950AA30AEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72314F88-94BB-A448-8F05-EBD75E68D461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" activeTab="7" xr2:uid="{146EE09F-7D4A-B94B-A812-6F28E341E2B6}"/>
+    <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" activeTab="8" xr2:uid="{146EE09F-7D4A-B94B-A812-6F28E341E2B6}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM-IDO" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="MHW" sheetId="7" r:id="rId6"/>
     <sheet name="UWA" sheetId="6" r:id="rId7"/>
     <sheet name="360E" sheetId="8" r:id="rId8"/>
+    <sheet name="HYD2O" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="148">
   <si>
     <t>AED ID</t>
   </si>
@@ -423,15 +424,6 @@
     <t>Lake Richmond Site 2</t>
   </si>
   <si>
-    <t>mhwLR-board</t>
-  </si>
-  <si>
-    <t>mhwLR-site2</t>
-  </si>
-  <si>
-    <t>LR-site2</t>
-  </si>
-  <si>
     <t>360eLR-board</t>
   </si>
   <si>
@@ -454,6 +446,48 @@
   </si>
   <si>
     <t>Assume logger is at the board?</t>
+  </si>
+  <si>
+    <t>LR1</t>
+  </si>
+  <si>
+    <t>LR2</t>
+  </si>
+  <si>
+    <t>mhwLR1</t>
+  </si>
+  <si>
+    <t>mhwLR2</t>
+  </si>
+  <si>
+    <t>EcoLR1</t>
+  </si>
+  <si>
+    <t>EcoLR2</t>
+  </si>
+  <si>
+    <t>EcoLR3</t>
+  </si>
+  <si>
+    <t>EcoLR4</t>
+  </si>
+  <si>
+    <t>hyd2oEcoLR1</t>
+  </si>
+  <si>
+    <t>hyd2oEcoLR2</t>
+  </si>
+  <si>
+    <t>hyd2oEcoLR3</t>
+  </si>
+  <si>
+    <t>hyd2oEcoLR4</t>
+  </si>
+  <si>
+    <t>Lake Richmond Site 3</t>
+  </si>
+  <si>
+    <t>Lake Richmond Site 4</t>
   </si>
 </sst>
 </file>
@@ -2563,7 +2597,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:J3"/>
+      <selection sqref="A1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2596,13 +2630,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>134</v>
       </c>
       <c r="C3" t="s">
         <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>134</v>
+      </c>
+      <c r="E3">
+        <v>378787</v>
+      </c>
+      <c r="F3">
+        <v>6427116</v>
       </c>
       <c r="J3" t="s">
         <v>123</v>
@@ -2610,13 +2653,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>135</v>
       </c>
       <c r="C4" t="s">
         <v>125</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>135</v>
+      </c>
+      <c r="E4">
+        <v>379059</v>
+      </c>
+      <c r="F4">
+        <v>6427057</v>
       </c>
       <c r="J4" t="s">
         <v>123</v>
@@ -2672,8 +2724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E30BBE7-7297-C54E-91E7-461CF34E11E3}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2706,7 +2758,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
         <v>111</v>
@@ -2718,37 +2770,173 @@
         <v>123</v>
       </c>
       <c r="K3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
-        <v>135</v>
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5332EFF-583A-6142-8D85-0D523529D9AD}">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3">
+        <v>379234</v>
+      </c>
+      <c r="F3">
+        <v>6426700</v>
+      </c>
+      <c r="J3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4">
+        <v>379055</v>
+      </c>
+      <c r="F4">
+        <v>6427391</v>
+      </c>
+      <c r="J4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5">
+        <v>378703</v>
+      </c>
+      <c r="F5">
+        <v>6427545</v>
+      </c>
+      <c r="J5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6">
+        <v>378806</v>
+      </c>
+      <c r="F6">
+        <v>6426899</v>
+      </c>
+      <c r="J6" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>